<commit_message>
improve handling of imports with source and non-empty rules store
</commit_message>
<xml_diff>
--- a/tests/data/pump_example.xlsx
+++ b/tests/data/pump_example.xlsx
@@ -609,7 +609,7 @@
     <t>logical</t>
   </si>
   <si>
-    <t>source</t>
+    <t>sourceId</t>
   </si>
   <si>
     <t>http://thisisneat.io/test</t>
@@ -622,7 +622,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -633,26 +633,32 @@
     <font>
       <b/>
       <sz val="20"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -737,12 +743,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -763,20 +772,23 @@
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1087,90 +1099,90 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="26.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="26.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>183</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>185</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>187</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="12" t="s">
         <v>189</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>190</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>192</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="13">
         <v>45638.46973379629</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="13">
         <v>45638.46973379629</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="14" t="s">
         <v>197</v>
       </c>
     </row>
@@ -1198,9 +1210,9 @@
     <col min="4" max="4" style="3" width="41.57642857142857" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="3" width="30.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="3" width="37.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="13.005" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="3" width="13.005" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="3" width="26.576428571428572" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="3" width="21.576428571428572" customWidth="1" bestFit="1"/>
@@ -1281,568 +1293,568 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="G3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5" t="s">
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6" t="s">
         <v>144</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="6" t="s">
+      <c r="G4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5" t="s">
+      <c r="J4" s="6"/>
+      <c r="K4" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5" t="s">
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6" t="s">
         <v>147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="6" t="s">
+      <c r="G5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5" t="s">
+      <c r="I5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5" t="s">
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6" t="s">
         <v>152</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="G7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7" t="s">
+      <c r="J7" s="8"/>
+      <c r="K7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7" t="s">
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8" t="s">
         <v>155</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="8" t="s">
+      <c r="G8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7" t="s">
+      <c r="J8" s="8"/>
+      <c r="K8" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7" t="s">
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8" t="s">
         <v>158</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7" t="s">
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8" t="s">
         <v>161</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="8" t="s">
+      <c r="G10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7" t="s">
+      <c r="J10" s="8"/>
+      <c r="K10" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7" t="s">
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8" t="s">
         <v>162</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6" t="s">
         <v>165</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="6" t="s">
+      <c r="G13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5" t="s">
+      <c r="J13" s="6"/>
+      <c r="K13" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5" t="s">
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6" t="s">
         <v>169</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="6" t="s">
+      <c r="G14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5" t="s">
+      <c r="J14" s="6"/>
+      <c r="K14" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5" t="s">
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6" t="s">
         <v>170</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5" t="s">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="6" t="s">
+      <c r="G15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5" t="s">
+      <c r="J15" s="6"/>
+      <c r="K15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5" t="s">
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6" t="s">
         <v>172</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="s">
+      <c r="D16" s="6"/>
+      <c r="E16" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="6" t="s">
+      <c r="G16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5" t="s">
+      <c r="J16" s="6"/>
+      <c r="K16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5" t="s">
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6" t="s">
         <v>174</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="6" t="s">
+      <c r="G17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5" t="s">
+      <c r="J17" s="6"/>
+      <c r="K17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5" t="s">
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6" t="s">
         <v>178</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5" t="s">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="G18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5" t="s">
+      <c r="J18" s="6"/>
+      <c r="K18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="L18" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5" t="s">
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1864,14 +1876,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="45.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="70.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="70.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="3" width="70.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="45.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="70.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="70.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="70.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -2588,12 +2600,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">

</xml_diff>

<commit_message>
Improve source entity update (#926)
* improve handling of imports with source and non-empty rules store

* fix issues
</commit_message>
<xml_diff>
--- a/tests/data/pump_example.xlsx
+++ b/tests/data/pump_example.xlsx
@@ -609,7 +609,7 @@
     <t>logical</t>
   </si>
   <si>
-    <t>source</t>
+    <t>sourceId</t>
   </si>
   <si>
     <t>http://thisisneat.io/test</t>
@@ -622,7 +622,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -633,26 +633,32 @@
     <font>
       <b/>
       <sz val="20"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -737,12 +743,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -763,20 +772,23 @@
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1087,90 +1099,90 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="26.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="26.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>183</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>185</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>187</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="12" t="s">
         <v>189</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>190</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>192</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="13">
         <v>45638.46973379629</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="13">
         <v>45638.46973379629</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="14" t="s">
         <v>197</v>
       </c>
     </row>
@@ -1198,9 +1210,9 @@
     <col min="4" max="4" style="3" width="41.57642857142857" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="3" width="30.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="3" width="37.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="13.005" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="3" width="13.005" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="3" width="26.576428571428572" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="3" width="21.576428571428572" customWidth="1" bestFit="1"/>
@@ -1281,568 +1293,568 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="G3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5" t="s">
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6" t="s">
         <v>144</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="6" t="s">
+      <c r="G4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5" t="s">
+      <c r="J4" s="6"/>
+      <c r="K4" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5" t="s">
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6" t="s">
         <v>147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="6" t="s">
+      <c r="G5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5" t="s">
+      <c r="I5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5" t="s">
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6" t="s">
         <v>152</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="G7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7" t="s">
+      <c r="J7" s="8"/>
+      <c r="K7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7" t="s">
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8" t="s">
         <v>155</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="8" t="s">
+      <c r="G8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7" t="s">
+      <c r="J8" s="8"/>
+      <c r="K8" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7" t="s">
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8" t="s">
         <v>158</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7" t="s">
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8" t="s">
         <v>161</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="8" t="s">
+      <c r="G10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7" t="s">
+      <c r="J10" s="8"/>
+      <c r="K10" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7" t="s">
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8" t="s">
         <v>162</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6" t="s">
         <v>165</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="6" t="s">
+      <c r="G13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5" t="s">
+      <c r="J13" s="6"/>
+      <c r="K13" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5" t="s">
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6" t="s">
         <v>169</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="6" t="s">
+      <c r="G14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5" t="s">
+      <c r="J14" s="6"/>
+      <c r="K14" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5" t="s">
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6" t="s">
         <v>170</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5" t="s">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="6" t="s">
+      <c r="G15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5" t="s">
+      <c r="J15" s="6"/>
+      <c r="K15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5" t="s">
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6" t="s">
         <v>172</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="s">
+      <c r="D16" s="6"/>
+      <c r="E16" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="6" t="s">
+      <c r="G16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5" t="s">
+      <c r="J16" s="6"/>
+      <c r="K16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5" t="s">
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6" t="s">
         <v>174</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="6" t="s">
+      <c r="G17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5" t="s">
+      <c r="J17" s="6"/>
+      <c r="K17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5" t="s">
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6" t="s">
         <v>178</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5" t="s">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="G18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5" t="s">
+      <c r="J18" s="6"/>
+      <c r="K18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="L18" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5" t="s">
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1864,14 +1876,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="45.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="70.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="70.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="3" width="70.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="45.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="70.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="70.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="70.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -2588,12 +2600,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">

</xml_diff>